<commit_message>
up modifiche per tracciamento e controtracciamento
</commit_message>
<xml_diff>
--- a/RQ/Esterni/Definizione di prodotto/Tracciamento Classi-requisiti.xlsx
+++ b/RQ/Esterni/Definizione di prodotto/Tracciamento Classi-requisiti.xlsx
@@ -13,7 +13,6 @@
     <sheet name="Formato Tabella" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -419,9 +418,6 @@
     <t>recupero</t>
   </si>
   <si>
-    <t>ROFB 9.1.1</t>
-  </si>
-  <si>
     <t>DT.V</t>
   </si>
   <si>
@@ -480,6 +476,9 @@
   </si>
   <si>
     <t>RFD  2.1</t>
+  </si>
+  <si>
+    <t>ROFB 9.1.2</t>
   </si>
 </sst>
 </file>
@@ -852,7 +851,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -924,7 +923,7 @@
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
@@ -1006,7 +1005,7 @@
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>11</v>
@@ -1114,7 +1113,7 @@
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>17</v>
@@ -1186,7 +1185,7 @@
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>18</v>
@@ -1258,7 +1257,7 @@
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>20</v>
@@ -1320,7 +1319,7 @@
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1">
       <c r="A47" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>21</v>
@@ -1422,7 +1421,7 @@
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1">
       <c r="A57" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>22</v>
@@ -1484,7 +1483,7 @@
     </row>
     <row r="63" spans="1:4" ht="15" customHeight="1">
       <c r="A63" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>93</v>
@@ -1543,7 +1542,7 @@
     </row>
     <row r="70" spans="1:4" ht="15" customHeight="1">
       <c r="A70" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>118</v>
@@ -1562,7 +1561,7 @@
     </row>
     <row r="72" spans="1:4" ht="15" customHeight="1">
       <c r="A72" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>88</v>
@@ -1662,7 +1661,7 @@
     </row>
     <row r="84" spans="1:4" ht="15" customHeight="1">
       <c r="A84" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>102</v>
@@ -1689,7 +1688,7 @@
     </row>
     <row r="87" spans="1:4" ht="15" customHeight="1">
       <c r="A87" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>9</v>
@@ -1732,8 +1731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G168"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -1747,7 +1746,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>121</v>
@@ -1860,7 +1859,7 @@
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>123</v>
@@ -1943,7 +1942,7 @@
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>122</v>
@@ -2074,13 +2073,13 @@
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>107</v>
@@ -2093,7 +2092,7 @@
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>124</v>
@@ -2168,7 +2167,7 @@
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>125</v>
@@ -2243,7 +2242,7 @@
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1">
       <c r="A56" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>119</v>
@@ -2262,7 +2261,7 @@
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>65</v>
@@ -2345,7 +2344,7 @@
     </row>
     <row r="68" spans="1:4" ht="15" customHeight="1">
       <c r="A68" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>66</v>
@@ -2452,7 +2451,7 @@
     </row>
     <row r="81" spans="1:4" ht="15" customHeight="1">
       <c r="A81" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>67</v>
@@ -2527,7 +2526,7 @@
     </row>
     <row r="90" spans="1:4" ht="15" customHeight="1">
       <c r="A90" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>120</v>
@@ -2602,7 +2601,7 @@
     </row>
     <row r="99" spans="1:4" ht="15" customHeight="1">
       <c r="A99" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>68</v>
@@ -2733,7 +2732,7 @@
     </row>
     <row r="115" spans="1:4" ht="15" customHeight="1">
       <c r="A115" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>69</v>
@@ -2808,7 +2807,7 @@
     </row>
     <row r="124" spans="1:4" ht="15" customHeight="1">
       <c r="A124" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>126</v>
@@ -2827,7 +2826,7 @@
     </row>
     <row r="126" spans="1:4" ht="15" customHeight="1">
       <c r="A126" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>127</v>
@@ -2841,7 +2840,7 @@
     </row>
     <row r="127" spans="1:4" ht="15" customHeight="1">
       <c r="C127" s="1" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>107</v>
@@ -2854,7 +2853,7 @@
     </row>
     <row r="129" spans="1:4" ht="15" customHeight="1">
       <c r="A129" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>128</v>
@@ -2868,7 +2867,7 @@
     </row>
     <row r="130" spans="1:4" ht="15" customHeight="1">
       <c r="C130" s="1" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>107</v>
@@ -2881,7 +2880,7 @@
     </row>
     <row r="132" spans="1:4" ht="15" customHeight="1">
       <c r="A132" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>70</v>
@@ -2932,7 +2931,7 @@
     </row>
     <row r="138" spans="1:4" ht="15" customHeight="1">
       <c r="A138" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>130</v>
@@ -2951,7 +2950,7 @@
     </row>
     <row r="140" spans="1:4" ht="15" customHeight="1">
       <c r="A140" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>130</v>
@@ -2986,7 +2985,7 @@
     </row>
     <row r="144" spans="1:4" ht="15" customHeight="1">
       <c r="A144" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>88</v>
@@ -3077,7 +3076,7 @@
     </row>
     <row r="155" spans="1:4" ht="15" customHeight="1">
       <c r="A155" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>87</v>
@@ -3104,13 +3103,13 @@
     </row>
     <row r="158" spans="1:4" ht="15" customHeight="1">
       <c r="A158" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>129</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D158" s="1" t="s">
         <v>107</v>
@@ -3154,13 +3153,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>107</v>
@@ -3168,7 +3167,7 @@
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1">
       <c r="C2" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>107</v>
@@ -3384,7 +3383,7 @@
     </row>
     <row r="29" spans="3:4" ht="15" customHeight="1">
       <c r="C29" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>107</v>
@@ -3392,7 +3391,7 @@
     </row>
     <row r="30" spans="3:4" ht="15" customHeight="1">
       <c r="C30" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>107</v>
@@ -3400,7 +3399,7 @@
     </row>
     <row r="31" spans="3:4" ht="15" customHeight="1">
       <c r="C31" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>107</v>
@@ -3408,7 +3407,7 @@
     </row>
     <row r="32" spans="3:4" ht="15" customHeight="1">
       <c r="C32" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>107</v>
@@ -3416,7 +3415,7 @@
     </row>
     <row r="33" spans="3:4" ht="15" customHeight="1">
       <c r="C33" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>107</v>
@@ -3472,7 +3471,7 @@
     </row>
     <row r="40" spans="3:4" ht="15" customHeight="1">
       <c r="C40" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>107</v>
@@ -3589,13 +3588,13 @@
     </row>
     <row r="55" spans="1:6" ht="15" customHeight="1">
       <c r="A55" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>109</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>107</v>
@@ -3603,7 +3602,7 @@
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1">
       <c r="C56" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>107</v>
@@ -3879,7 +3878,7 @@
     </row>
     <row r="88" spans="1:6" ht="15" customHeight="1">
       <c r="A88" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>72</v>
@@ -3906,7 +3905,7 @@
     </row>
     <row r="91" spans="1:6" ht="15" customHeight="1">
       <c r="A91" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>74</v>
@@ -3949,7 +3948,7 @@
     </row>
     <row r="96" spans="1:6" ht="15" customHeight="1">
       <c r="A96" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>76</v>
@@ -4049,7 +4048,7 @@
     </row>
     <row r="108" spans="1:4" ht="15" customHeight="1">
       <c r="A108" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>77</v>
@@ -4101,7 +4100,7 @@
     </row>
     <row r="114" spans="1:4" ht="15" customHeight="1">
       <c r="A114" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>78</v>
@@ -4128,7 +4127,7 @@
     </row>
     <row r="117" spans="1:4" ht="15" customHeight="1">
       <c r="A117" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>79</v>
@@ -4150,7 +4149,7 @@
     </row>
     <row r="119" spans="1:4" ht="15" customHeight="1">
       <c r="C119" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>107</v>
@@ -4163,7 +4162,7 @@
     </row>
     <row r="121" spans="1:4" ht="15" customHeight="1">
       <c r="A121" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>80</v>
@@ -4238,7 +4237,7 @@
     </row>
     <row r="130" spans="1:4" ht="15" customHeight="1">
       <c r="A130" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>81</v>
@@ -4260,7 +4259,7 @@
     </row>
     <row r="132" spans="1:4" ht="15" customHeight="1">
       <c r="C132" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>107</v>
@@ -4268,7 +4267,7 @@
     </row>
     <row r="133" spans="1:4" ht="15" customHeight="1">
       <c r="C133" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>107</v>
@@ -4276,7 +4275,7 @@
     </row>
     <row r="134" spans="1:4" ht="15" customHeight="1">
       <c r="C134" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>107</v>
@@ -4284,7 +4283,7 @@
     </row>
     <row r="135" spans="1:4" ht="15" customHeight="1">
       <c r="C135" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>107</v>
@@ -4292,7 +4291,7 @@
     </row>
     <row r="136" spans="1:4" ht="15" customHeight="1">
       <c r="C136" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D136" s="1" t="s">
         <v>107</v>
@@ -4321,13 +4320,13 @@
     </row>
     <row r="140" spans="1:4" ht="15" customHeight="1">
       <c r="A140" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>103</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>107</v>
@@ -4335,7 +4334,7 @@
     </row>
     <row r="141" spans="1:4" ht="15" customHeight="1">
       <c r="C141" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>107</v>
@@ -4364,7 +4363,7 @@
     </row>
     <row r="145" spans="1:4" ht="15" customHeight="1">
       <c r="A145" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>110</v>
@@ -4391,7 +4390,7 @@
     </row>
     <row r="148" spans="1:4" ht="15" customHeight="1">
       <c r="A148" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>91</v>
@@ -4426,13 +4425,13 @@
     </row>
     <row r="152" spans="1:4" ht="15" customHeight="1">
       <c r="A152" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>94</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D152" s="1" t="s">
         <v>107</v>
@@ -4440,7 +4439,7 @@
     </row>
     <row r="153" spans="1:4" ht="15" customHeight="1">
       <c r="C153" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D153" s="1" t="s">
         <v>107</v>
@@ -4648,7 +4647,7 @@
     </row>
     <row r="179" spans="3:4" ht="15" customHeight="1">
       <c r="C179" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D179" s="1" t="s">
         <v>107</v>
@@ -4656,7 +4655,7 @@
     </row>
     <row r="180" spans="3:4" ht="15" customHeight="1">
       <c r="C180" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D180" s="1" t="s">
         <v>107</v>
@@ -4664,7 +4663,7 @@
     </row>
     <row r="181" spans="3:4" ht="15" customHeight="1">
       <c r="C181" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D181" s="1" t="s">
         <v>107</v>
@@ -4672,7 +4671,7 @@
     </row>
     <row r="182" spans="3:4" ht="15" customHeight="1">
       <c r="C182" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D182" s="1" t="s">
         <v>107</v>
@@ -4680,7 +4679,7 @@
     </row>
     <row r="183" spans="3:4" ht="15" customHeight="1">
       <c r="C183" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D183" s="1" t="s">
         <v>107</v>
@@ -4789,7 +4788,7 @@
     </row>
     <row r="197" spans="1:4" ht="15" customHeight="1">
       <c r="A197" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>95</v>
@@ -4832,7 +4831,7 @@
     </row>
     <row r="202" spans="1:4" ht="15" customHeight="1">
       <c r="A202" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>97</v>
@@ -4875,7 +4874,7 @@
     </row>
     <row r="207" spans="1:4" ht="15" customHeight="1">
       <c r="A207" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>96</v>
@@ -4910,7 +4909,7 @@
     </row>
     <row r="211" spans="1:4" ht="15" customHeight="1">
       <c r="A211" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>98</v>
@@ -4964,7 +4963,7 @@
     </row>
     <row r="217" spans="1:4" ht="15" customHeight="1">
       <c r="C217" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D217" s="1" t="s">
         <v>107</v>
@@ -5004,7 +5003,7 @@
     </row>
     <row r="222" spans="1:4" ht="15" customHeight="1">
       <c r="C222" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D222" s="1" t="s">
         <v>107</v>
@@ -5017,7 +5016,7 @@
     </row>
     <row r="224" spans="1:4" ht="15" customHeight="1">
       <c r="A224" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B224" s="1" t="s">
         <v>99</v>
@@ -5117,7 +5116,7 @@
     </row>
     <row r="236" spans="1:4" ht="15" customHeight="1">
       <c r="A236" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B236" s="1" t="s">
         <v>100</v>
@@ -5144,7 +5143,7 @@
     </row>
     <row r="239" spans="1:4" ht="15" customHeight="1">
       <c r="A239" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B239" s="1" t="s">
         <v>104</v>
@@ -5171,7 +5170,7 @@
     </row>
     <row r="242" spans="1:4" ht="15" customHeight="1">
       <c r="A242" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B242" s="1" t="s">
         <v>115</v>
@@ -5206,7 +5205,7 @@
     </row>
     <row r="246" spans="1:4" ht="15" customHeight="1">
       <c r="A246" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B246" s="1" t="s">
         <v>114</v>
@@ -5260,7 +5259,7 @@
     </row>
     <row r="252" spans="1:4" ht="15" customHeight="1">
       <c r="C252" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D252" s="1" t="s">
         <v>107</v>
@@ -5300,7 +5299,7 @@
     </row>
     <row r="257" spans="1:4" ht="15" customHeight="1">
       <c r="C257" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D257" s="1" t="s">
         <v>107</v>
@@ -5313,7 +5312,7 @@
     </row>
     <row r="259" spans="1:4" ht="15" customHeight="1">
       <c r="A259" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B259" s="1" t="s">
         <v>113</v>
@@ -5413,7 +5412,7 @@
     </row>
     <row r="271" spans="1:4" ht="15" customHeight="1">
       <c r="A271" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>112</v>
@@ -5440,7 +5439,7 @@
     </row>
     <row r="274" spans="1:4" ht="15" customHeight="1">
       <c r="A274" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B274" s="1" t="s">
         <v>111</v>
@@ -5467,7 +5466,7 @@
     </row>
     <row r="277" spans="1:4" ht="15" customHeight="1">
       <c r="A277" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B277" s="1" t="s">
         <v>84</v>
@@ -5518,7 +5517,7 @@
     </row>
     <row r="283" spans="1:4" ht="15" customHeight="1">
       <c r="A283" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B283" s="1" t="s">
         <v>101</v>
@@ -5545,7 +5544,7 @@
     </row>
     <row r="286" spans="1:4" ht="15" customHeight="1">
       <c r="A286" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B286" s="1" t="s">
         <v>9</v>
@@ -5580,7 +5579,7 @@
     </row>
     <row r="290" spans="1:4" ht="15" customHeight="1">
       <c r="A290" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B290" s="1" t="s">
         <v>90</v>
@@ -5616,7 +5615,7 @@
     </row>
     <row r="294" spans="1:4" ht="15" customHeight="1">
       <c r="A294" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B294" s="1" t="s">
         <v>89</v>
@@ -5707,7 +5706,7 @@
     </row>
     <row r="305" spans="1:4" ht="15" customHeight="1">
       <c r="A305" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B305" s="1" t="s">
         <v>88</v>
@@ -5807,7 +5806,7 @@
     </row>
     <row r="317" spans="1:4" ht="15" customHeight="1">
       <c r="A317" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B317" s="1" t="s">
         <v>102</v>
@@ -5834,7 +5833,7 @@
     </row>
     <row r="320" spans="1:4" ht="15" customHeight="1">
       <c r="A320" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B320" s="1" t="s">
         <v>105</v>
@@ -5877,7 +5876,7 @@
     </row>
     <row r="325" spans="1:6" ht="15" customHeight="1">
       <c r="A325" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B325" s="1" t="s">
         <v>116</v>
@@ -5896,7 +5895,7 @@
     </row>
     <row r="327" spans="1:6" ht="15" customHeight="1">
       <c r="A327" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B327" s="1" t="s">
         <v>117</v>
@@ -6164,7 +6163,7 @@
     </row>
     <row r="359" spans="3:7" ht="15" customHeight="1">
       <c r="C359" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D359" s="1" t="s">
         <v>107</v>
@@ -6172,7 +6171,7 @@
     </row>
     <row r="360" spans="3:7" ht="15" customHeight="1">
       <c r="C360" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D360" s="1" t="s">
         <v>107</v>
@@ -6180,7 +6179,7 @@
     </row>
     <row r="361" spans="3:7" ht="15" customHeight="1">
       <c r="C361" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D361" s="1" t="s">
         <v>107</v>
@@ -6188,7 +6187,7 @@
     </row>
     <row r="362" spans="3:7" ht="15" customHeight="1">
       <c r="C362" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D362" s="1" t="s">
         <v>107</v>
@@ -6196,7 +6195,7 @@
     </row>
     <row r="363" spans="3:7" ht="15" customHeight="1">
       <c r="C363" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D363" s="1" t="s">
         <v>107</v>
@@ -6253,7 +6252,7 @@
     </row>
     <row r="370" spans="3:4" ht="15" customHeight="1">
       <c r="C370" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D370" s="1" t="s">
         <v>107</v>
@@ -6365,7 +6364,7 @@
     </row>
     <row r="384" spans="3:4" ht="15" customHeight="1">
       <c r="C384" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D384" s="1" t="s">
         <v>107</v>

</xml_diff>

<commit_message>
un tracciamento e piccola modifica ar
</commit_message>
<xml_diff>
--- a/RQ/Esterni/Definizione di prodotto/Tracciamento Classi-requisiti.xlsx
+++ b/RQ/Esterni/Definizione di prodotto/Tracciamento Classi-requisiti.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="154">
   <si>
     <t>Requisito</t>
   </si>
@@ -839,7 +839,7 @@
   <dimension ref="A1:D90"/>
   <sheetViews>
     <sheetView topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90"/>
+      <selection activeCell="D11" sqref="A3:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -1729,10 +1729,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G168"/>
+  <dimension ref="A1:G170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59:C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -2274,16 +2274,16 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1">
-      <c r="C59" s="1" t="s">
-        <v>4</v>
+      <c r="C59" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1">
-      <c r="C60" s="1" t="s">
-        <v>5</v>
+      <c r="C60" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>107</v>
@@ -2291,7 +2291,7 @@
     </row>
     <row r="61" spans="1:4" ht="15" customHeight="1">
       <c r="C61" s="1" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>107</v>
@@ -2299,7 +2299,7 @@
     </row>
     <row r="62" spans="1:4" ht="15" customHeight="1">
       <c r="C62" s="1" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>107</v>
@@ -2307,7 +2307,7 @@
     </row>
     <row r="63" spans="1:4" ht="15" customHeight="1">
       <c r="C63" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>107</v>
@@ -2315,7 +2315,7 @@
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1">
       <c r="C64" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>107</v>
@@ -2323,7 +2323,7 @@
     </row>
     <row r="65" spans="1:4" ht="15" customHeight="1">
       <c r="C65" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>107</v>
@@ -2331,42 +2331,42 @@
     </row>
     <row r="66" spans="1:4" ht="15" customHeight="1">
       <c r="C66" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15" customHeight="1">
+      <c r="C67" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15" customHeight="1">
+      <c r="C68" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="15" customHeight="1">
-      <c r="D67" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="15" customHeight="1">
-      <c r="A68" s="1" t="s">
+      <c r="D68" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15" customHeight="1">
+      <c r="D69" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15" customHeight="1">
+      <c r="A70" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C70" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="15" customHeight="1">
-      <c r="C69" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="15" customHeight="1">
-      <c r="C70" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>107</v>
@@ -2374,7 +2374,7 @@
     </row>
     <row r="71" spans="1:4" ht="15" customHeight="1">
       <c r="C71" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>107</v>
@@ -2382,7 +2382,7 @@
     </row>
     <row r="72" spans="1:4" ht="15" customHeight="1">
       <c r="C72" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>107</v>
@@ -2390,23 +2390,23 @@
     </row>
     <row r="73" spans="1:4" ht="15" customHeight="1">
       <c r="C73" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="15" customHeight="1">
+      <c r="C74" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="15" customHeight="1">
+      <c r="C75" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="15" customHeight="1">
-      <c r="C74" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="15" customHeight="1">
-      <c r="C75" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>107</v>
@@ -2414,7 +2414,7 @@
     </row>
     <row r="76" spans="1:4" ht="15" customHeight="1">
       <c r="C76" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>107</v>
@@ -2422,7 +2422,7 @@
     </row>
     <row r="77" spans="1:4" ht="15" customHeight="1">
       <c r="C77" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>107</v>
@@ -2430,7 +2430,7 @@
     </row>
     <row r="78" spans="1:4" ht="15" customHeight="1">
       <c r="C78" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>107</v>
@@ -2438,50 +2438,50 @@
     </row>
     <row r="79" spans="1:4" ht="15" customHeight="1">
       <c r="C79" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="15" customHeight="1">
+      <c r="C80" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="15" customHeight="1">
+      <c r="C81" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D79" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="15" customHeight="1">
-      <c r="D80" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="15" customHeight="1">
-      <c r="A81" s="1" t="s">
+      <c r="D81" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="15" customHeight="1">
+      <c r="D82" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="15" customHeight="1">
+      <c r="A83" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B83" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="C83" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D81" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="15" customHeight="1">
-      <c r="C82" s="3" t="s">
+      <c r="D83" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="15" customHeight="1">
+      <c r="C84" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="15" customHeight="1">
-      <c r="C83" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="15" customHeight="1">
-      <c r="C84" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>107</v>
@@ -2489,7 +2489,7 @@
     </row>
     <row r="85" spans="1:4" ht="15" customHeight="1">
       <c r="C85" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>107</v>
@@ -2497,7 +2497,7 @@
     </row>
     <row r="86" spans="1:4" ht="15" customHeight="1">
       <c r="C86" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>107</v>
@@ -2505,7 +2505,7 @@
     </row>
     <row r="87" spans="1:4" ht="15" customHeight="1">
       <c r="C87" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>107</v>
@@ -2513,50 +2513,50 @@
     </row>
     <row r="88" spans="1:4" ht="15" customHeight="1">
       <c r="C88" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="15" customHeight="1">
+      <c r="C89" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="15" customHeight="1">
+      <c r="C90" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D88" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="15" customHeight="1">
-      <c r="D89" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="15" customHeight="1">
-      <c r="A90" s="1" t="s">
+      <c r="D90" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="15" customHeight="1">
+      <c r="D91" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="15" customHeight="1">
+      <c r="A92" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B92" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C90" s="3" t="s">
+      <c r="C92" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D90" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="15" customHeight="1">
-      <c r="C91" s="3" t="s">
+      <c r="D92" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="15" customHeight="1">
+      <c r="C93" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="15" customHeight="1">
-      <c r="C92" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="15" customHeight="1">
-      <c r="C93" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>107</v>
@@ -2564,7 +2564,7 @@
     </row>
     <row r="94" spans="1:4" ht="15" customHeight="1">
       <c r="C94" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>107</v>
@@ -2572,7 +2572,7 @@
     </row>
     <row r="95" spans="1:4" ht="15" customHeight="1">
       <c r="C95" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>107</v>
@@ -2580,7 +2580,7 @@
     </row>
     <row r="96" spans="1:4" ht="15" customHeight="1">
       <c r="C96" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>107</v>
@@ -2588,42 +2588,42 @@
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1">
       <c r="C97" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="15" customHeight="1">
+      <c r="C98" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="15" customHeight="1">
+      <c r="C99" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D97" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="15" customHeight="1">
-      <c r="D98" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="15" customHeight="1">
-      <c r="A99" s="1" t="s">
+      <c r="D99" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="15" customHeight="1">
+      <c r="D100" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="15" customHeight="1">
+      <c r="A101" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C101" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" ht="15" customHeight="1">
-      <c r="C100" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" ht="15" customHeight="1">
-      <c r="C101" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>107</v>
@@ -2631,7 +2631,7 @@
     </row>
     <row r="102" spans="1:4" ht="15" customHeight="1">
       <c r="C102" s="3" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>107</v>
@@ -2639,7 +2639,7 @@
     </row>
     <row r="103" spans="1:4" ht="15" customHeight="1">
       <c r="C103" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>107</v>
@@ -2647,7 +2647,7 @@
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1">
       <c r="C104" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>107</v>
@@ -2655,7 +2655,7 @@
     </row>
     <row r="105" spans="1:4" ht="15" customHeight="1">
       <c r="C105" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>107</v>
@@ -2663,7 +2663,7 @@
     </row>
     <row r="106" spans="1:4" ht="15" customHeight="1">
       <c r="C106" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>107</v>
@@ -2671,23 +2671,23 @@
     </row>
     <row r="107" spans="1:4" ht="15" customHeight="1">
       <c r="C107" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="15" customHeight="1">
+      <c r="C108" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="15" customHeight="1">
+      <c r="C109" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="15" customHeight="1">
-      <c r="C108" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" ht="15" customHeight="1">
-      <c r="C109" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>107</v>
@@ -2695,7 +2695,7 @@
     </row>
     <row r="110" spans="1:4" ht="15" customHeight="1">
       <c r="C110" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>107</v>
@@ -2703,7 +2703,7 @@
     </row>
     <row r="111" spans="1:4" ht="15" customHeight="1">
       <c r="C111" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>107</v>
@@ -2711,7 +2711,7 @@
     </row>
     <row r="112" spans="1:4" ht="15" customHeight="1">
       <c r="C112" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>107</v>
@@ -2719,50 +2719,50 @@
     </row>
     <row r="113" spans="1:4" ht="15" customHeight="1">
       <c r="C113" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="15" customHeight="1">
+      <c r="C114" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="15" customHeight="1">
+      <c r="C115" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D113" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="15" customHeight="1">
-      <c r="D114" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" ht="15" customHeight="1">
-      <c r="A115" s="1" t="s">
+      <c r="D115" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="15" customHeight="1">
+      <c r="D116" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="15" customHeight="1">
+      <c r="A117" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B117" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C115" s="3" t="s">
+      <c r="C117" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D115" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" ht="15" customHeight="1">
-      <c r="C116" s="3" t="s">
+      <c r="D117" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="15" customHeight="1">
+      <c r="C118" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" ht="15" customHeight="1">
-      <c r="C117" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="15" customHeight="1">
-      <c r="C118" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>107</v>
@@ -2770,7 +2770,7 @@
     </row>
     <row r="119" spans="1:4" ht="15" customHeight="1">
       <c r="C119" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>107</v>
@@ -2778,7 +2778,7 @@
     </row>
     <row r="120" spans="1:4" ht="15" customHeight="1">
       <c r="C120" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>107</v>
@@ -2786,7 +2786,7 @@
     </row>
     <row r="121" spans="1:4" ht="15" customHeight="1">
       <c r="C121" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>107</v>
@@ -2794,26 +2794,23 @@
     </row>
     <row r="122" spans="1:4" ht="15" customHeight="1">
       <c r="C122" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="15" customHeight="1">
+      <c r="C123" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="15" customHeight="1">
+      <c r="C124" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="15" customHeight="1">
-      <c r="D123" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="15" customHeight="1">
-      <c r="A124" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>107</v>
@@ -2829,115 +2826,115 @@
         <v>137</v>
       </c>
       <c r="B126" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="15" customHeight="1">
+      <c r="D127" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="15" customHeight="1">
+      <c r="A128" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B128" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C126" s="1" t="s">
+      <c r="C128" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D126" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" ht="15" customHeight="1">
-      <c r="C127" s="1" t="s">
+      <c r="D128" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="15" customHeight="1">
+      <c r="C129" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D127" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" ht="15" customHeight="1">
-      <c r="D128" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" ht="15" customHeight="1">
-      <c r="A129" s="1" t="s">
+      <c r="D129" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="15" customHeight="1">
+      <c r="D130" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="15" customHeight="1">
+      <c r="A131" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B129" s="1" t="s">
+      <c r="B131" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="C131" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D129" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" ht="15" customHeight="1">
-      <c r="C130" s="1" t="s">
+      <c r="D131" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="15" customHeight="1">
+      <c r="C132" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D130" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" ht="15" customHeight="1">
-      <c r="D131" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" ht="15" customHeight="1">
-      <c r="A132" s="1" t="s">
+      <c r="D132" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="15" customHeight="1">
+      <c r="D133" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="15" customHeight="1">
+      <c r="A134" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="B134" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C132" s="3" t="s">
+      <c r="C134" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D132" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" ht="15" customHeight="1">
-      <c r="C133" s="3" t="s">
+      <c r="D134" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="15" customHeight="1">
+      <c r="C135" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D133" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" ht="15" customHeight="1">
-      <c r="C134" s="3" t="s">
+      <c r="D135" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="15" customHeight="1">
+      <c r="C136" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D134" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" ht="15" customHeight="1">
-      <c r="C135" s="1" t="s">
+      <c r="D136" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="15" customHeight="1">
+      <c r="C137" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D135" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" ht="15" customHeight="1">
-      <c r="C136" s="1" t="s">
+      <c r="D137" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="15" customHeight="1">
+      <c r="C138" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" ht="15" customHeight="1">
-      <c r="D137" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" ht="15" customHeight="1">
-      <c r="A138" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="D138" s="1" t="s">
         <v>107</v>
@@ -2956,58 +2953,61 @@
         <v>130</v>
       </c>
       <c r="C140" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="15" customHeight="1">
+      <c r="D141" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" ht="15" customHeight="1">
+      <c r="A142" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C142" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D140" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" ht="15" customHeight="1">
-      <c r="C141" s="1" t="s">
+      <c r="D142" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="15" customHeight="1">
+      <c r="C143" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D141" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" ht="15" customHeight="1">
-      <c r="C142" s="1" t="s">
+      <c r="D143" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="15" customHeight="1">
+      <c r="C144" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D142" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" ht="15" customHeight="1">
-      <c r="D143" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" ht="15" customHeight="1">
-      <c r="A144" s="1" t="s">
+      <c r="D144" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="15" customHeight="1">
+      <c r="D145" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="15" customHeight="1">
+      <c r="A146" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B144" s="1" t="s">
+      <c r="B146" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C144" s="3" t="s">
+      <c r="C146" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="D144" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" ht="15" customHeight="1">
-      <c r="C145" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D145" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" ht="15" customHeight="1">
-      <c r="C146" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="D146" s="1" t="s">
         <v>107</v>
@@ -3015,7 +3015,7 @@
     </row>
     <row r="147" spans="1:4" ht="15" customHeight="1">
       <c r="C147" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D147" s="1" t="s">
         <v>107</v>
@@ -3023,7 +3023,7 @@
     </row>
     <row r="148" spans="1:4" ht="15" customHeight="1">
       <c r="C148" s="3" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="D148" s="1" t="s">
         <v>107</v>
@@ -3031,7 +3031,7 @@
     </row>
     <row r="149" spans="1:4" ht="15" customHeight="1">
       <c r="C149" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>107</v>
@@ -3039,7 +3039,7 @@
     </row>
     <row r="150" spans="1:4" ht="15" customHeight="1">
       <c r="C150" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>107</v>
@@ -3047,69 +3047,66 @@
     </row>
     <row r="151" spans="1:4" ht="15" customHeight="1">
       <c r="C151" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="15" customHeight="1">
+      <c r="C152" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="15" customHeight="1">
+      <c r="C153" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D151" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" ht="15" customHeight="1">
-      <c r="C152" s="1" t="s">
+      <c r="D153" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="15" customHeight="1">
+      <c r="C154" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D152" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" ht="15" customHeight="1">
-      <c r="C153" s="1" t="s">
+      <c r="D154" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="15" customHeight="1">
+      <c r="C155" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D153" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" ht="15" customHeight="1">
-      <c r="D154" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" ht="15" customHeight="1">
-      <c r="A155" s="1" t="s">
+      <c r="D155" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="15" customHeight="1">
+      <c r="D156" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="15" customHeight="1">
+      <c r="A157" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B155" s="1" t="s">
+      <c r="B157" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C155" s="1" t="s">
+      <c r="C157" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D155" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" ht="15" customHeight="1">
-      <c r="C156" s="1" t="s">
+      <c r="D157" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="15" customHeight="1">
+      <c r="C158" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" ht="15" customHeight="1">
-      <c r="D157" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" ht="15" customHeight="1">
-      <c r="A158" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="D158" s="1" t="s">
         <v>107</v>
@@ -3120,11 +3117,30 @@
         <v>108</v>
       </c>
     </row>
-    <row r="167" spans="3:3" ht="15" customHeight="1">
-      <c r="C167" s="3"/>
-    </row>
-    <row r="168" spans="3:3" ht="15" customHeight="1">
-      <c r="C168" s="3"/>
+    <row r="160" spans="1:4" ht="15" customHeight="1">
+      <c r="A160" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="161" spans="3:4" ht="15" customHeight="1">
+      <c r="D161" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="169" spans="3:4" ht="15" customHeight="1">
+      <c r="C169" s="3"/>
+    </row>
+    <row r="170" spans="3:4" ht="15" customHeight="1">
+      <c r="C170" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
90% tracciamento e controtracciamento
</commit_message>
<xml_diff>
--- a/RQ/Esterni/Definizione di prodotto/Tracciamento Classi-requisiti.xlsx
+++ b/RQ/Esterni/Definizione di prodotto/Tracciamento Classi-requisiti.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="10515" windowHeight="7485" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="10515" windowHeight="7485" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Desktop" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="153">
   <si>
     <t>Requisito</t>
   </si>
@@ -413,9 +413,6 @@
   </si>
   <si>
     <t>DomandaActivity.QuestTask</t>
-  </si>
-  <si>
-    <t>recupero</t>
   </si>
   <si>
     <t>DT.V</t>
@@ -508,7 +505,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -516,32 +513,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -851,7 +831,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -923,7 +903,7 @@
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
@@ -1005,7 +985,7 @@
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>11</v>
@@ -1113,7 +1093,7 @@
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>17</v>
@@ -1185,7 +1165,7 @@
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>18</v>
@@ -1257,7 +1237,7 @@
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>20</v>
@@ -1319,7 +1299,7 @@
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1">
       <c r="A47" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>21</v>
@@ -1421,7 +1401,7 @@
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1">
       <c r="A57" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>22</v>
@@ -1483,7 +1463,7 @@
     </row>
     <row r="63" spans="1:4" ht="15" customHeight="1">
       <c r="A63" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>93</v>
@@ -1542,7 +1522,7 @@
     </row>
     <row r="70" spans="1:4" ht="15" customHeight="1">
       <c r="A70" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>118</v>
@@ -1561,7 +1541,7 @@
     </row>
     <row r="72" spans="1:4" ht="15" customHeight="1">
       <c r="A72" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>88</v>
@@ -1661,7 +1641,7 @@
     </row>
     <row r="84" spans="1:4" ht="15" customHeight="1">
       <c r="A84" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>102</v>
@@ -1688,7 +1668,7 @@
     </row>
     <row r="87" spans="1:4" ht="15" customHeight="1">
       <c r="A87" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>9</v>
@@ -1729,10 +1709,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G170"/>
+  <dimension ref="A1:G169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59:C60"/>
+    <sheetView topLeftCell="A133" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B141" sqref="A141:B141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -1746,7 +1726,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>121</v>
@@ -1757,12 +1737,8 @@
       <c r="D1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1">
       <c r="C2" s="3" t="s">
@@ -1771,10 +1747,8 @@
       <c r="D2" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1">
       <c r="C3" s="1" t="s">
@@ -1783,10 +1757,8 @@
       <c r="D3" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1">
       <c r="C4" s="1" t="s">
@@ -1795,10 +1767,8 @@
       <c r="D4" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
-        <v>64</v>
-      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1">
       <c r="C5" s="1" t="s">
@@ -1807,10 +1777,8 @@
       <c r="D5" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4" t="s">
-        <v>61</v>
-      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1">
       <c r="C6" s="1" t="s">
@@ -1819,10 +1787,8 @@
       <c r="D6" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4" t="s">
-        <v>62</v>
-      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1">
       <c r="C7" s="1" t="s">
@@ -1831,10 +1797,8 @@
       <c r="D7" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1">
       <c r="C8" s="1" t="s">
@@ -1843,23 +1807,19 @@
       <c r="D8" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4" t="s">
-        <v>71</v>
-      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1">
       <c r="D9" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>123</v>
@@ -1942,7 +1902,7 @@
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>122</v>
@@ -2073,7 +2033,7 @@
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>131</v>
@@ -2092,7 +2052,7 @@
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>124</v>
@@ -2167,7 +2127,7 @@
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>125</v>
@@ -2242,7 +2202,7 @@
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1">
       <c r="A56" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>119</v>
@@ -2261,7 +2221,7 @@
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>65</v>
@@ -2360,7 +2320,7 @@
     </row>
     <row r="70" spans="1:4" ht="15" customHeight="1">
       <c r="A70" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>66</v>
@@ -2467,7 +2427,7 @@
     </row>
     <row r="83" spans="1:4" ht="15" customHeight="1">
       <c r="A83" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>67</v>
@@ -2542,7 +2502,7 @@
     </row>
     <row r="92" spans="1:4" ht="15" customHeight="1">
       <c r="A92" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>120</v>
@@ -2617,7 +2577,7 @@
     </row>
     <row r="101" spans="1:4" ht="15" customHeight="1">
       <c r="A101" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>68</v>
@@ -2748,7 +2708,7 @@
     </row>
     <row r="117" spans="1:4" ht="15" customHeight="1">
       <c r="A117" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>69</v>
@@ -2823,7 +2783,7 @@
     </row>
     <row r="126" spans="1:4" ht="15" customHeight="1">
       <c r="A126" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>126</v>
@@ -2842,7 +2802,7 @@
     </row>
     <row r="128" spans="1:4" ht="15" customHeight="1">
       <c r="A128" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>127</v>
@@ -2856,7 +2816,7 @@
     </row>
     <row r="129" spans="1:4" ht="15" customHeight="1">
       <c r="C129" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>107</v>
@@ -2869,7 +2829,7 @@
     </row>
     <row r="131" spans="1:4" ht="15" customHeight="1">
       <c r="A131" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>128</v>
@@ -2883,7 +2843,7 @@
     </row>
     <row r="132" spans="1:4" ht="15" customHeight="1">
       <c r="C132" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>107</v>
@@ -2896,7 +2856,7 @@
     </row>
     <row r="134" spans="1:4" ht="15" customHeight="1">
       <c r="A134" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>70</v>
@@ -2947,7 +2907,7 @@
     </row>
     <row r="140" spans="1:4" ht="15" customHeight="1">
       <c r="A140" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>130</v>
@@ -2960,19 +2920,16 @@
       </c>
     </row>
     <row r="141" spans="1:4" ht="15" customHeight="1">
+      <c r="C141" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D141" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="15" customHeight="1">
-      <c r="A142" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B142" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="C142" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>107</v>
@@ -2980,34 +2937,34 @@
     </row>
     <row r="143" spans="1:4" ht="15" customHeight="1">
       <c r="C143" s="1" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="D143" s="1" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="15" customHeight="1">
-      <c r="C144" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="D144" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="15" customHeight="1">
+      <c r="A145" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="D145" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="15" customHeight="1">
-      <c r="A146" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="C146" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D146" s="1" t="s">
         <v>107</v>
@@ -3015,7 +2972,7 @@
     </row>
     <row r="147" spans="1:4" ht="15" customHeight="1">
       <c r="C147" s="3" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="D147" s="1" t="s">
         <v>107</v>
@@ -3023,7 +2980,7 @@
     </row>
     <row r="148" spans="1:4" ht="15" customHeight="1">
       <c r="C148" s="3" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="D148" s="1" t="s">
         <v>107</v>
@@ -3031,7 +2988,7 @@
     </row>
     <row r="149" spans="1:4" ht="15" customHeight="1">
       <c r="C149" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>107</v>
@@ -3039,7 +2996,7 @@
     </row>
     <row r="150" spans="1:4" ht="15" customHeight="1">
       <c r="C150" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>107</v>
@@ -3047,7 +3004,7 @@
     </row>
     <row r="151" spans="1:4" ht="15" customHeight="1">
       <c r="C151" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>107</v>
@@ -3055,15 +3012,15 @@
     </row>
     <row r="152" spans="1:4" ht="15" customHeight="1">
       <c r="C152" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D152" s="1" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="15" customHeight="1">
-      <c r="C153" s="3" t="s">
-        <v>39</v>
+      <c r="C153" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="D153" s="1" t="s">
         <v>107</v>
@@ -3071,76 +3028,68 @@
     </row>
     <row r="154" spans="1:4" ht="15" customHeight="1">
       <c r="C154" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D154" s="1" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="15" customHeight="1">
-      <c r="C155" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="D155" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="15" customHeight="1">
+      <c r="A156" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D156" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="15" customHeight="1">
-      <c r="A157" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="C157" s="1" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="D157" s="1" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="15" customHeight="1">
-      <c r="C158" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="D158" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="15" customHeight="1">
+      <c r="A159" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="D159" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="15" customHeight="1">
-      <c r="A160" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="D160" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="161" spans="3:4" ht="15" customHeight="1">
-      <c r="D161" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="169" spans="3:4" ht="15" customHeight="1">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="168" spans="3:3" ht="15" customHeight="1">
+      <c r="C168" s="3"/>
+    </row>
+    <row r="169" spans="3:3" ht="15" customHeight="1">
       <c r="C169" s="3"/>
-    </row>
-    <row r="170" spans="3:4" ht="15" customHeight="1">
-      <c r="C170" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3152,8 +3101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G390"/>
   <sheetViews>
-    <sheetView topLeftCell="A360" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D390"/>
+    <sheetView tabSelected="1" topLeftCell="A202" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E202" sqref="E202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -3169,13 +3118,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>107</v>
@@ -3183,7 +3132,7 @@
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1">
       <c r="C2" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>107</v>
@@ -3399,7 +3348,7 @@
     </row>
     <row r="29" spans="3:4" ht="15" customHeight="1">
       <c r="C29" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>107</v>
@@ -3407,7 +3356,7 @@
     </row>
     <row r="30" spans="3:4" ht="15" customHeight="1">
       <c r="C30" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>107</v>
@@ -3415,7 +3364,7 @@
     </row>
     <row r="31" spans="3:4" ht="15" customHeight="1">
       <c r="C31" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>107</v>
@@ -3423,7 +3372,7 @@
     </row>
     <row r="32" spans="3:4" ht="15" customHeight="1">
       <c r="C32" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>107</v>
@@ -3431,7 +3380,7 @@
     </row>
     <row r="33" spans="3:4" ht="15" customHeight="1">
       <c r="C33" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>107</v>
@@ -3487,7 +3436,7 @@
     </row>
     <row r="40" spans="3:4" ht="15" customHeight="1">
       <c r="C40" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>107</v>
@@ -3604,13 +3553,13 @@
     </row>
     <row r="55" spans="1:6" ht="15" customHeight="1">
       <c r="A55" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>109</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>107</v>
@@ -3618,7 +3567,7 @@
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1">
       <c r="C56" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>107</v>
@@ -3894,7 +3843,7 @@
     </row>
     <row r="88" spans="1:6" ht="15" customHeight="1">
       <c r="A88" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>72</v>
@@ -3921,7 +3870,7 @@
     </row>
     <row r="91" spans="1:6" ht="15" customHeight="1">
       <c r="A91" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>74</v>
@@ -3964,7 +3913,7 @@
     </row>
     <row r="96" spans="1:6" ht="15" customHeight="1">
       <c r="A96" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>76</v>
@@ -4064,7 +4013,7 @@
     </row>
     <row r="108" spans="1:4" ht="15" customHeight="1">
       <c r="A108" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>77</v>
@@ -4116,7 +4065,7 @@
     </row>
     <row r="114" spans="1:4" ht="15" customHeight="1">
       <c r="A114" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>78</v>
@@ -4143,7 +4092,7 @@
     </row>
     <row r="117" spans="1:4" ht="15" customHeight="1">
       <c r="A117" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>79</v>
@@ -4165,7 +4114,7 @@
     </row>
     <row r="119" spans="1:4" ht="15" customHeight="1">
       <c r="C119" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>107</v>
@@ -4178,7 +4127,7 @@
     </row>
     <row r="121" spans="1:4" ht="15" customHeight="1">
       <c r="A121" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>80</v>
@@ -4253,7 +4202,7 @@
     </row>
     <row r="130" spans="1:4" ht="15" customHeight="1">
       <c r="A130" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>81</v>
@@ -4275,7 +4224,7 @@
     </row>
     <row r="132" spans="1:4" ht="15" customHeight="1">
       <c r="C132" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>107</v>
@@ -4283,7 +4232,7 @@
     </row>
     <row r="133" spans="1:4" ht="15" customHeight="1">
       <c r="C133" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>107</v>
@@ -4291,7 +4240,7 @@
     </row>
     <row r="134" spans="1:4" ht="15" customHeight="1">
       <c r="C134" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>107</v>
@@ -4299,7 +4248,7 @@
     </row>
     <row r="135" spans="1:4" ht="15" customHeight="1">
       <c r="C135" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>107</v>
@@ -4307,7 +4256,7 @@
     </row>
     <row r="136" spans="1:4" ht="15" customHeight="1">
       <c r="C136" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D136" s="1" t="s">
         <v>107</v>
@@ -4336,13 +4285,13 @@
     </row>
     <row r="140" spans="1:4" ht="15" customHeight="1">
       <c r="A140" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>103</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>107</v>
@@ -4350,7 +4299,7 @@
     </row>
     <row r="141" spans="1:4" ht="15" customHeight="1">
       <c r="C141" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>107</v>
@@ -4379,7 +4328,7 @@
     </row>
     <row r="145" spans="1:4" ht="15" customHeight="1">
       <c r="A145" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>110</v>
@@ -4406,7 +4355,7 @@
     </row>
     <row r="148" spans="1:4" ht="15" customHeight="1">
       <c r="A148" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>91</v>
@@ -4441,13 +4390,13 @@
     </row>
     <row r="152" spans="1:4" ht="15" customHeight="1">
       <c r="A152" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>94</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D152" s="1" t="s">
         <v>107</v>
@@ -4455,7 +4404,7 @@
     </row>
     <row r="153" spans="1:4" ht="15" customHeight="1">
       <c r="C153" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D153" s="1" t="s">
         <v>107</v>
@@ -4663,7 +4612,7 @@
     </row>
     <row r="179" spans="3:4" ht="15" customHeight="1">
       <c r="C179" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D179" s="1" t="s">
         <v>107</v>
@@ -4671,7 +4620,7 @@
     </row>
     <row r="180" spans="3:4" ht="15" customHeight="1">
       <c r="C180" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D180" s="1" t="s">
         <v>107</v>
@@ -4679,7 +4628,7 @@
     </row>
     <row r="181" spans="3:4" ht="15" customHeight="1">
       <c r="C181" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D181" s="1" t="s">
         <v>107</v>
@@ -4687,7 +4636,7 @@
     </row>
     <row r="182" spans="3:4" ht="15" customHeight="1">
       <c r="C182" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D182" s="1" t="s">
         <v>107</v>
@@ -4695,7 +4644,7 @@
     </row>
     <row r="183" spans="3:4" ht="15" customHeight="1">
       <c r="C183" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D183" s="1" t="s">
         <v>107</v>
@@ -4804,7 +4753,7 @@
     </row>
     <row r="197" spans="1:4" ht="15" customHeight="1">
       <c r="A197" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>95</v>
@@ -4847,7 +4796,7 @@
     </row>
     <row r="202" spans="1:4" ht="15" customHeight="1">
       <c r="A202" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>97</v>
@@ -4890,7 +4839,7 @@
     </row>
     <row r="207" spans="1:4" ht="15" customHeight="1">
       <c r="A207" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>96</v>
@@ -4925,7 +4874,7 @@
     </row>
     <row r="211" spans="1:4" ht="15" customHeight="1">
       <c r="A211" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>98</v>
@@ -4979,7 +4928,7 @@
     </row>
     <row r="217" spans="1:4" ht="15" customHeight="1">
       <c r="C217" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D217" s="1" t="s">
         <v>107</v>
@@ -5019,7 +4968,7 @@
     </row>
     <row r="222" spans="1:4" ht="15" customHeight="1">
       <c r="C222" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D222" s="1" t="s">
         <v>107</v>
@@ -5032,7 +4981,7 @@
     </row>
     <row r="224" spans="1:4" ht="15" customHeight="1">
       <c r="A224" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B224" s="1" t="s">
         <v>99</v>
@@ -5132,7 +5081,7 @@
     </row>
     <row r="236" spans="1:4" ht="15" customHeight="1">
       <c r="A236" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B236" s="1" t="s">
         <v>100</v>
@@ -5159,7 +5108,7 @@
     </row>
     <row r="239" spans="1:4" ht="15" customHeight="1">
       <c r="A239" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B239" s="1" t="s">
         <v>104</v>
@@ -5186,7 +5135,7 @@
     </row>
     <row r="242" spans="1:4" ht="15" customHeight="1">
       <c r="A242" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B242" s="1" t="s">
         <v>115</v>
@@ -5221,7 +5170,7 @@
     </row>
     <row r="246" spans="1:4" ht="15" customHeight="1">
       <c r="A246" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B246" s="1" t="s">
         <v>114</v>
@@ -5275,7 +5224,7 @@
     </row>
     <row r="252" spans="1:4" ht="15" customHeight="1">
       <c r="C252" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D252" s="1" t="s">
         <v>107</v>
@@ -5315,7 +5264,7 @@
     </row>
     <row r="257" spans="1:4" ht="15" customHeight="1">
       <c r="C257" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D257" s="1" t="s">
         <v>107</v>
@@ -5328,7 +5277,7 @@
     </row>
     <row r="259" spans="1:4" ht="15" customHeight="1">
       <c r="A259" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B259" s="1" t="s">
         <v>113</v>
@@ -5428,7 +5377,7 @@
     </row>
     <row r="271" spans="1:4" ht="15" customHeight="1">
       <c r="A271" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>112</v>
@@ -5455,7 +5404,7 @@
     </row>
     <row r="274" spans="1:4" ht="15" customHeight="1">
       <c r="A274" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B274" s="1" t="s">
         <v>111</v>
@@ -5482,7 +5431,7 @@
     </row>
     <row r="277" spans="1:4" ht="15" customHeight="1">
       <c r="A277" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B277" s="1" t="s">
         <v>84</v>
@@ -5533,7 +5482,7 @@
     </row>
     <row r="283" spans="1:4" ht="15" customHeight="1">
       <c r="A283" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B283" s="1" t="s">
         <v>101</v>
@@ -5560,7 +5509,7 @@
     </row>
     <row r="286" spans="1:4" ht="15" customHeight="1">
       <c r="A286" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B286" s="1" t="s">
         <v>9</v>
@@ -5595,7 +5544,7 @@
     </row>
     <row r="290" spans="1:4" ht="15" customHeight="1">
       <c r="A290" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B290" s="1" t="s">
         <v>90</v>
@@ -5631,7 +5580,7 @@
     </row>
     <row r="294" spans="1:4" ht="15" customHeight="1">
       <c r="A294" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B294" s="1" t="s">
         <v>89</v>
@@ -5722,7 +5671,7 @@
     </row>
     <row r="305" spans="1:4" ht="15" customHeight="1">
       <c r="A305" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B305" s="1" t="s">
         <v>88</v>
@@ -5822,7 +5771,7 @@
     </row>
     <row r="317" spans="1:4" ht="15" customHeight="1">
       <c r="A317" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B317" s="1" t="s">
         <v>102</v>
@@ -5849,7 +5798,7 @@
     </row>
     <row r="320" spans="1:4" ht="15" customHeight="1">
       <c r="A320" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B320" s="1" t="s">
         <v>105</v>
@@ -5892,7 +5841,7 @@
     </row>
     <row r="325" spans="1:6" ht="15" customHeight="1">
       <c r="A325" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B325" s="1" t="s">
         <v>116</v>
@@ -5911,7 +5860,7 @@
     </row>
     <row r="327" spans="1:6" ht="15" customHeight="1">
       <c r="A327" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B327" s="1" t="s">
         <v>117</v>
@@ -6179,7 +6128,7 @@
     </row>
     <row r="359" spans="3:7" ht="15" customHeight="1">
       <c r="C359" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D359" s="1" t="s">
         <v>107</v>
@@ -6187,7 +6136,7 @@
     </row>
     <row r="360" spans="3:7" ht="15" customHeight="1">
       <c r="C360" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D360" s="1" t="s">
         <v>107</v>
@@ -6195,7 +6144,7 @@
     </row>
     <row r="361" spans="3:7" ht="15" customHeight="1">
       <c r="C361" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D361" s="1" t="s">
         <v>107</v>
@@ -6203,7 +6152,7 @@
     </row>
     <row r="362" spans="3:7" ht="15" customHeight="1">
       <c r="C362" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D362" s="1" t="s">
         <v>107</v>
@@ -6211,7 +6160,7 @@
     </row>
     <row r="363" spans="3:7" ht="15" customHeight="1">
       <c r="C363" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D363" s="1" t="s">
         <v>107</v>
@@ -6268,7 +6217,7 @@
     </row>
     <row r="370" spans="3:4" ht="15" customHeight="1">
       <c r="C370" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D370" s="1" t="s">
         <v>107</v>
@@ -6380,7 +6329,7 @@
     </row>
     <row r="384" spans="3:4" ht="15" customHeight="1">
       <c r="C384" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D384" s="1" t="s">
         <v>107</v>

</xml_diff>